<commit_message>
Update the correct week
</commit_message>
<xml_diff>
--- a/Sufficient data WITH_PO/forecast_summary_B083RVN2VG_WITH_PO.xlsx
+++ b/Sufficient data WITH_PO/forecast_summary_B083RVN2VG_WITH_PO.xlsx
@@ -512,7 +512,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>W1</t>
+          <t>W05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>1.13</v>
+        <v>1.01</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -581,7 +581,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>W06</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>1.08</v>
+        <v>1.2</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -650,7 +650,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W07</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -708,7 +708,7 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>0.97</v>
+        <v>0.91</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
@@ -719,7 +719,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="P5" t="n">
-        <v>0.9</v>
+        <v>1.08</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -788,7 +788,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>W5</t>
+          <t>W09</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -846,7 +846,7 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>1.1</v>
+        <v>1.12</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>W6</t>
+          <t>W10</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>1.17</v>
+        <v>1.02</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
@@ -926,7 +926,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>W7</t>
+          <t>W11</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="n">
         <v>87</v>
@@ -984,7 +984,7 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>0.98</v>
+        <v>1.03</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -995,7 +995,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W8</t>
+          <t>W12</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="P9" t="n">
-        <v>1.19</v>
+        <v>0.96</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
@@ -1064,7 +1064,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>W9</t>
+          <t>W13</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>1.08</v>
+        <v>1.17</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1133,7 +1133,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>W10</t>
+          <t>W14</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1191,7 +1191,7 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>1.1</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -1202,7 +1202,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>W11</t>
+          <t>W15</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1216,7 +1216,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" t="n">
         <v>85</v>
@@ -1260,7 +1260,7 @@
         </is>
       </c>
       <c r="P12" t="n">
-        <v>1.15</v>
+        <v>0.89</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
@@ -1271,7 +1271,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>W12</t>
+          <t>W16</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E13" t="n">
         <v>81</v>
@@ -1329,7 +1329,7 @@
         </is>
       </c>
       <c r="P13" t="n">
-        <v>1.06</v>
+        <v>0.99</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>W13</t>
+          <t>W17</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1398,7 +1398,7 @@
         </is>
       </c>
       <c r="P14" t="n">
-        <v>1.02</v>
+        <v>1.06</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
@@ -1409,7 +1409,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>W14</t>
+          <t>W18</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1478,7 +1478,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>W15</t>
+          <t>W19</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1536,7 +1536,7 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>0.92</v>
+        <v>0.82</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
@@ -1547,7 +1547,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>W16</t>
+          <t>W20</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1561,7 +1561,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E17" t="n">
         <v>78</v>
@@ -1605,7 +1605,7 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>1.18</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>849</t>
         </is>
       </c>
     </row>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>69</t>
         </is>
       </c>
     </row>

</xml_diff>